<commit_message>
404 error, temp 14-32 coast
</commit_message>
<xml_diff>
--- a/SLC.xlsx
+++ b/SLC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WACKE\Desktop\saflink\flight-review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9A7278-FFF8-418D-8709-72ED02EBDE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5013ED-15B5-440D-AD48-BA874429F66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIL" sheetId="2" r:id="rId1"/>
@@ -96,7 +96,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -134,11 +134,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -148,6 +161,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC89A66-016F-4B05-8368-42ED2AD95DEE}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -586,10 +600,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H4"/>
+      <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -597,33 +611,42 @@
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="9">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9">
+        <v>16</v>
+      </c>
+      <c r="D1" s="9">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2">
         <v>20</v>
       </c>
-      <c r="C1" s="2">
+      <c r="F1" s="2">
         <v>22</v>
       </c>
-      <c r="D1" s="2">
+      <c r="G1" s="2">
         <v>24</v>
       </c>
-      <c r="E1" s="2">
+      <c r="H1" s="2">
         <v>26</v>
       </c>
-      <c r="F1" s="2">
+      <c r="I1" s="2">
         <v>28</v>
       </c>
-      <c r="G1" s="2">
+      <c r="J1" s="2">
         <v>30</v>
       </c>
-      <c r="H1" s="2">
+      <c r="K1" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -648,8 +671,17 @@
       <c r="H2" s="2">
         <v>43000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75">
+      <c r="I2" s="2">
+        <v>43000</v>
+      </c>
+      <c r="J2" s="2">
+        <v>43000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -674,8 +706,17 @@
       <c r="H3" s="4">
         <v>43000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75">
+      <c r="I3" s="4">
+        <v>43000</v>
+      </c>
+      <c r="J3" s="4">
+        <v>43000</v>
+      </c>
+      <c r="K3" s="4">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,6 +739,15 @@
         <v>43000</v>
       </c>
       <c r="H4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="J4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="K4" s="2">
         <v>43000</v>
       </c>
     </row>
@@ -708,41 +758,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6854CBAE-708D-4DAE-85C4-2C4413AFA3B6}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H4"/>
+      <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="9">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9">
+        <v>16</v>
+      </c>
+      <c r="D1" s="9">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2">
         <v>20</v>
       </c>
-      <c r="C1" s="2">
+      <c r="F1" s="2">
         <v>22</v>
       </c>
-      <c r="D1" s="2">
+      <c r="G1" s="2">
         <v>24</v>
       </c>
-      <c r="E1" s="2">
+      <c r="H1" s="2">
         <v>26</v>
       </c>
-      <c r="F1" s="2">
+      <c r="I1" s="2">
         <v>28</v>
       </c>
-      <c r="G1" s="2">
+      <c r="J1" s="2">
         <v>30</v>
       </c>
-      <c r="H1" s="2">
+      <c r="K1" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -767,8 +826,17 @@
       <c r="H2" s="2">
         <v>43000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75">
+      <c r="I2" s="2">
+        <v>43000</v>
+      </c>
+      <c r="J2" s="2">
+        <v>43000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -793,8 +861,17 @@
       <c r="H3" s="4">
         <v>43000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75">
+      <c r="I3" s="4">
+        <v>43000</v>
+      </c>
+      <c r="J3" s="4">
+        <v>43000</v>
+      </c>
+      <c r="K3" s="4">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,6 +894,15 @@
         <v>43000</v>
       </c>
       <c r="H4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="J4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="K4" s="2">
         <v>43000</v>
       </c>
     </row>
@@ -827,41 +913,50 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DB39F5-90AC-46DD-9925-E3F6A0E25A59}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H4"/>
+      <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="9">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9">
+        <v>16</v>
+      </c>
+      <c r="D1" s="9">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2">
         <v>20</v>
       </c>
-      <c r="C1" s="2">
+      <c r="F1" s="2">
         <v>22</v>
       </c>
-      <c r="D1" s="2">
+      <c r="G1" s="2">
         <v>24</v>
       </c>
-      <c r="E1" s="2">
+      <c r="H1" s="2">
         <v>26</v>
       </c>
-      <c r="F1" s="2">
+      <c r="I1" s="2">
         <v>28</v>
       </c>
-      <c r="G1" s="2">
+      <c r="J1" s="2">
         <v>30</v>
       </c>
-      <c r="H1" s="2">
+      <c r="K1" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -886,8 +981,17 @@
       <c r="H2" s="2">
         <v>43000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75">
+      <c r="I2" s="2">
+        <v>43000</v>
+      </c>
+      <c r="J2" s="2">
+        <v>43000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -912,8 +1016,17 @@
       <c r="H3" s="4">
         <v>43000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75">
+      <c r="I3" s="4">
+        <v>43000</v>
+      </c>
+      <c r="J3" s="4">
+        <v>43000</v>
+      </c>
+      <c r="K3" s="4">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,6 +1049,15 @@
         <v>43000</v>
       </c>
       <c r="H4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="J4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="K4" s="2">
         <v>43000</v>
       </c>
     </row>
@@ -946,41 +1068,50 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6567EA82-C83D-4048-8E7F-C388B194B793}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="9">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9">
+        <v>16</v>
+      </c>
+      <c r="D1" s="9">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2">
         <v>20</v>
       </c>
-      <c r="C1" s="2">
+      <c r="F1" s="2">
         <v>22</v>
       </c>
-      <c r="D1" s="2">
+      <c r="G1" s="2">
         <v>24</v>
       </c>
-      <c r="E1" s="2">
+      <c r="H1" s="2">
         <v>26</v>
       </c>
-      <c r="F1" s="2">
+      <c r="I1" s="2">
         <v>28</v>
       </c>
-      <c r="G1" s="2">
+      <c r="J1" s="2">
         <v>30</v>
       </c>
-      <c r="H1" s="2">
+      <c r="K1" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1005,8 +1136,17 @@
       <c r="H2" s="2">
         <v>43000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75">
+      <c r="I2" s="2">
+        <v>43000</v>
+      </c>
+      <c r="J2" s="2">
+        <v>43000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1031,8 +1171,17 @@
       <c r="H3" s="4">
         <v>43000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75">
+      <c r="I3" s="4">
+        <v>43000</v>
+      </c>
+      <c r="J3" s="4">
+        <v>43000</v>
+      </c>
+      <c r="K3" s="4">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1055,6 +1204,15 @@
         <v>43000</v>
       </c>
       <c r="H4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="J4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="K4" s="2">
         <v>43000</v>
       </c>
     </row>

</xml_diff>